<commit_message>
fichier excel non remplir
</commit_message>
<xml_diff>
--- a/exercice1.xlsx
+++ b/exercice1.xlsx
@@ -674,9 +674,7 @@
           <t>Bénéfice optimal</t>
         </is>
       </c>
-      <c r="B1" t="n">
-        <v>952</v>
-      </c>
+      <c r="B1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -751,66 +749,26 @@
           <t>Chargé (0/1)</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>1</v>
-      </c>
-      <c r="O3" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>1</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" t="n">
-        <v>1</v>
-      </c>
-      <c r="T3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U3" t="n">
-        <v>0</v>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>